<commit_message>
Added Sources and Targets
</commit_message>
<xml_diff>
--- a/song-data-collection/0. Manually Collected Metahpor Data.xlsx
+++ b/song-data-collection/0. Manually Collected Metahpor Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mashk\MyFiles\Semester 7\CS4642 - Data Mining &amp; Information Retrieval\IR-Mini-Project\repo\song-data-collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0E45F4-34B4-4525-A3BF-27C083A5C2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED5B51F-9E12-49C5-91C7-39C560300BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="634">
   <si>
     <t>ID</t>
   </si>
@@ -1812,66 +1812,6 @@
   </si>
   <si>
     <t>kirilliya</t>
-  </si>
-  <si>
-    <t>{T}, {S} men sundara nisa yodha atha</t>
-  </si>
-  <si>
-    <t>somyaya</t>
-  </si>
-  <si>
-    <t>mihiriya</t>
-  </si>
-  <si>
-    <t>manaramya</t>
-  </si>
-  <si>
-    <t>sithkaluya</t>
-  </si>
-  <si>
-    <t>dakumakaluya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adhala awasthawedi {T} hi katuka bawa agawai </t>
-  </si>
-  <si>
-    <t>{T} hi watinakama penweemata yodha atha</t>
-  </si>
-  <si>
-    <t>{T} hi wishalathwaya penweemata yodha atha</t>
-  </si>
-  <si>
-    <t>{T} loku pitiwahalak bawa penweemata</t>
-  </si>
-  <si>
-    <t>{T} loku hayyak bawa penweemata</t>
-  </si>
-  <si>
-    <t>{T} loku Udawwak bawa penweemata</t>
-  </si>
-  <si>
-    <t>{T} himi nowana bawa penweemata</t>
-  </si>
-  <si>
-    <t>{T} wihiluwak wee athi bawa penweemata</t>
-  </si>
-  <si>
-    <t>baila geeyak nisa arthayak natha</t>
-  </si>
-  <si>
-    <t>wiyawaharaye yedena wachanayaki</t>
-  </si>
-  <si>
-    <t>{T} ikmanin nathiweema penwi</t>
-  </si>
-  <si>
-    <t>{T} hi kreeyasheeli, chnachala bawa agawai</t>
-  </si>
-  <si>
-    <t>{T} , {U} men siyum yay agawai</t>
-  </si>
-  <si>
-    <t>{T} hi thrupthimath bawa agawai</t>
   </si>
   <si>
     <t>Name</t>
@@ -2601,8 +2541,8 @@
   </sheetPr>
   <dimension ref="A1:AD998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView tabSelected="1" topLeftCell="E209" workbookViewId="0">
+      <selection activeCell="G232" sqref="G232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2622,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -2672,7 +2612,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
@@ -2681,7 +2621,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -2749,7 +2689,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>615</v>
+        <v>595</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>20</v>
@@ -2778,7 +2718,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>616</v>
+        <v>596</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>24</v>
@@ -2816,7 +2756,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -2836,7 +2776,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>617</v>
+        <v>597</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>33</v>
@@ -3018,7 +2958,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>618</v>
+        <v>598</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>54</v>
@@ -3543,7 +3483,7 @@
         <v>120</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
@@ -3899,7 +3839,7 @@
         <v>27</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>160</v>
@@ -4167,7 +4107,7 @@
         <v>31</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>186</v>
@@ -4299,7 +4239,7 @@
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="6" t="s">
-        <v>644</v>
+        <v>624</v>
       </c>
       <c r="F70" s="7">
         <v>1</v>
@@ -4453,7 +4393,7 @@
         <v>37</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>213</v>
@@ -4625,7 +4565,7 @@
         <v>231</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>646</v>
+        <v>626</v>
       </c>
       <c r="F84" s="7">
         <v>1</v>
@@ -4913,7 +4853,7 @@
         <v>262</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
       <c r="F96" s="7">
         <v>1</v>
@@ -5124,7 +5064,7 @@
         <v>285</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>647</v>
+        <v>627</v>
       </c>
       <c r="F105" s="7">
         <v>1</v>
@@ -5240,7 +5180,7 @@
         <v>53</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="C110" s="11" t="s">
         <v>298</v>
@@ -5278,7 +5218,7 @@
         <v>304</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>648</v>
+        <v>628</v>
       </c>
       <c r="F111" s="7">
         <v>1</v>
@@ -5394,7 +5334,7 @@
         <v>57</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>318</v>
@@ -5423,7 +5363,7 @@
         <v>58</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>624</v>
+        <v>604</v>
       </c>
       <c r="C117" s="11" t="s">
         <v>322</v>
@@ -5490,7 +5430,7 @@
         <v>59</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>625</v>
+        <v>605</v>
       </c>
       <c r="C120" s="11" t="s">
         <v>325</v>
@@ -5528,7 +5468,7 @@
         <v>330</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
       <c r="F121" s="7">
         <v>1</v>
@@ -5584,7 +5524,7 @@
       </c>
       <c r="D123" s="6"/>
       <c r="E123" s="6" t="s">
-        <v>652</v>
+        <v>632</v>
       </c>
       <c r="F123" s="7">
         <v>1</v>
@@ -6020,7 +5960,7 @@
         <v>71</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>626</v>
+        <v>606</v>
       </c>
       <c r="C142" s="11" t="s">
         <v>384</v>
@@ -6029,7 +5969,7 @@
         <v>385</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>649</v>
+        <v>629</v>
       </c>
       <c r="F142" s="7">
         <v>1</v>
@@ -6096,7 +6036,7 @@
         <v>390</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F145" s="7">
         <v>1</v>
@@ -6135,7 +6075,7 @@
         <v>73</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="C147" s="11" t="s">
         <v>393</v>
@@ -6144,7 +6084,7 @@
         <v>394</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>651</v>
+        <v>631</v>
       </c>
       <c r="F147" s="7">
         <v>1</v>
@@ -6164,7 +6104,7 @@
         <v>74</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>628</v>
+        <v>608</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>397</v>
@@ -6442,7 +6382,7 @@
         <v>79</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>629</v>
+        <v>609</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>424</v>
@@ -6499,7 +6439,7 @@
         <v>432</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>653</v>
+        <v>633</v>
       </c>
       <c r="F162" s="7">
         <v>1</v>
@@ -6557,7 +6497,7 @@
         <v>81</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>630</v>
+        <v>610</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>436</v>
@@ -6566,7 +6506,7 @@
         <v>437</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>643</v>
+        <v>623</v>
       </c>
       <c r="F165" s="7">
         <v>1</v>
@@ -6776,7 +6716,7 @@
         <v>86</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>631</v>
+        <v>611</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>463</v>
@@ -6908,7 +6848,7 @@
         <v>88</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>632</v>
+        <v>612</v>
       </c>
       <c r="C180" s="11" t="s">
         <v>475</v>
@@ -6917,7 +6857,7 @@
         <v>476</v>
       </c>
       <c r="E180" s="6" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
       <c r="F180" s="7">
         <v>1</v>
@@ -6994,7 +6934,7 @@
         <v>89</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>633</v>
+        <v>613</v>
       </c>
       <c r="C184" s="11" t="s">
         <v>479</v>
@@ -7071,7 +7011,7 @@
         <v>91</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>634</v>
+        <v>614</v>
       </c>
       <c r="C187" s="11" t="s">
         <v>489</v>
@@ -7128,7 +7068,7 @@
         <v>496</v>
       </c>
       <c r="E189" s="6" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
       <c r="F189" s="7">
         <v>1</v>
@@ -7167,7 +7107,7 @@
         <v>93</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>635</v>
+        <v>615</v>
       </c>
       <c r="C191" s="11" t="s">
         <v>498</v>
@@ -7176,7 +7116,7 @@
         <v>499</v>
       </c>
       <c r="E191" s="6" t="s">
-        <v>645</v>
+        <v>625</v>
       </c>
       <c r="F191" s="7">
         <v>1</v>
@@ -7242,7 +7182,7 @@
         <v>95</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>636</v>
+        <v>616</v>
       </c>
       <c r="C194" s="11" t="s">
         <v>504</v>
@@ -7463,7 +7403,7 @@
         <v>100</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>637</v>
+        <v>617</v>
       </c>
       <c r="C203" s="11" t="s">
         <v>531</v>
@@ -7559,7 +7499,7 @@
         <v>102</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>638</v>
+        <v>618</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>540</v>
@@ -7844,7 +7784,7 @@
         <v>106</v>
       </c>
       <c r="B220" s="47" t="s">
-        <v>639</v>
+        <v>619</v>
       </c>
       <c r="C220" s="11" t="s">
         <v>566</v>
@@ -7997,7 +7937,7 @@
         <v>108</v>
       </c>
       <c r="B227" s="47" t="s">
-        <v>640</v>
+        <v>620</v>
       </c>
       <c r="C227" s="11" t="s">
         <v>578</v>
@@ -8074,7 +8014,7 @@
         <v>110</v>
       </c>
       <c r="B230" s="47" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>587</v>
@@ -8166,10 +8106,7 @@
         <f>COUNTBLANK(D2:D233) -122</f>
         <v>10</v>
       </c>
-      <c r="I235" s="7">
-        <f>COUNTBLANK(I2:I233)</f>
-        <v>0</v>
-      </c>
+      <c r="I235" s="7"/>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="3"/>
@@ -8184,12 +8121,8 @@
       <c r="C237" s="9"/>
       <c r="D237" s="6"/>
       <c r="E237" s="6"/>
-      <c r="F237" s="7">
-        <v>1</v>
-      </c>
-      <c r="G237" s="7" t="s">
-        <v>593</v>
-      </c>
+      <c r="F237" s="7"/>
+      <c r="G237" s="7"/>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="3"/>
@@ -8197,9 +8130,7 @@
       <c r="C238" s="9"/>
       <c r="D238" s="6"/>
       <c r="E238" s="6"/>
-      <c r="G238" s="7" t="s">
-        <v>594</v>
-      </c>
+      <c r="G238" s="7"/>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="3"/>
@@ -8207,9 +8138,7 @@
       <c r="C239" s="9"/>
       <c r="D239" s="6"/>
       <c r="E239" s="6"/>
-      <c r="G239" s="7" t="s">
-        <v>595</v>
-      </c>
+      <c r="G239" s="7"/>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
@@ -8217,9 +8146,7 @@
       <c r="C240" s="9"/>
       <c r="D240" s="6"/>
       <c r="E240" s="6"/>
-      <c r="G240" s="7" t="s">
-        <v>596</v>
-      </c>
+      <c r="G240" s="7"/>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="3"/>
@@ -8227,9 +8154,7 @@
       <c r="C241" s="9"/>
       <c r="D241" s="6"/>
       <c r="E241" s="6"/>
-      <c r="G241" s="7" t="s">
-        <v>597</v>
-      </c>
+      <c r="G241" s="7"/>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="3"/>
@@ -8237,9 +8162,7 @@
       <c r="C242" s="9"/>
       <c r="D242" s="6"/>
       <c r="E242" s="6"/>
-      <c r="G242" s="7" t="s">
-        <v>598</v>
-      </c>
+      <c r="G242" s="7"/>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
@@ -8254,12 +8177,8 @@
       <c r="C244" s="9"/>
       <c r="D244" s="6"/>
       <c r="E244" s="6"/>
-      <c r="F244" s="7">
-        <v>2</v>
-      </c>
-      <c r="G244" s="7" t="s">
-        <v>599</v>
-      </c>
+      <c r="F244" s="7"/>
+      <c r="G244" s="7"/>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
@@ -8267,12 +8186,8 @@
       <c r="C245" s="9"/>
       <c r="D245" s="6"/>
       <c r="E245" s="6"/>
-      <c r="F245" s="7">
-        <v>3</v>
-      </c>
-      <c r="G245" s="7" t="s">
-        <v>600</v>
-      </c>
+      <c r="F245" s="7"/>
+      <c r="G245" s="7"/>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
@@ -8280,12 +8195,8 @@
       <c r="C246" s="9"/>
       <c r="D246" s="6"/>
       <c r="E246" s="6"/>
-      <c r="F246" s="7">
-        <v>4</v>
-      </c>
-      <c r="G246" s="7" t="s">
-        <v>601</v>
-      </c>
+      <c r="F246" s="7"/>
+      <c r="G246" s="7"/>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
@@ -8293,12 +8204,8 @@
       <c r="C247" s="9"/>
       <c r="D247" s="6"/>
       <c r="E247" s="6"/>
-      <c r="F247" s="7">
-        <v>5</v>
-      </c>
-      <c r="G247" s="7" t="s">
-        <v>602</v>
-      </c>
+      <c r="F247" s="7"/>
+      <c r="G247" s="7"/>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="3"/>
@@ -8306,9 +8213,7 @@
       <c r="C248" s="9"/>
       <c r="D248" s="6"/>
       <c r="E248" s="6"/>
-      <c r="G248" s="7" t="s">
-        <v>603</v>
-      </c>
+      <c r="G248" s="7"/>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
@@ -8316,9 +8221,7 @@
       <c r="C249" s="9"/>
       <c r="D249" s="6"/>
       <c r="E249" s="6"/>
-      <c r="G249" s="7" t="s">
-        <v>604</v>
-      </c>
+      <c r="G249" s="7"/>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="3"/>
@@ -8333,12 +8236,8 @@
       <c r="C251" s="9"/>
       <c r="D251" s="6"/>
       <c r="E251" s="6"/>
-      <c r="F251" s="7">
-        <v>6</v>
-      </c>
-      <c r="G251" s="7" t="s">
-        <v>605</v>
-      </c>
+      <c r="F251" s="7"/>
+      <c r="G251" s="7"/>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="3"/>
@@ -8346,12 +8245,8 @@
       <c r="C252" s="9"/>
       <c r="D252" s="6"/>
       <c r="E252" s="6"/>
-      <c r="F252" s="7">
-        <v>7</v>
-      </c>
-      <c r="G252" s="7" t="s">
-        <v>606</v>
-      </c>
+      <c r="F252" s="7"/>
+      <c r="G252" s="7"/>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="3"/>
@@ -8359,12 +8254,8 @@
       <c r="C253" s="9"/>
       <c r="D253" s="6"/>
       <c r="E253" s="6"/>
-      <c r="F253" s="7">
-        <v>8</v>
-      </c>
-      <c r="G253" s="7" t="s">
-        <v>607</v>
-      </c>
+      <c r="F253" s="7"/>
+      <c r="G253" s="7"/>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="3"/>
@@ -8372,12 +8263,8 @@
       <c r="C254" s="9"/>
       <c r="D254" s="6"/>
       <c r="E254" s="6"/>
-      <c r="F254" s="7">
-        <v>9</v>
-      </c>
-      <c r="G254" s="7" t="s">
-        <v>608</v>
-      </c>
+      <c r="F254" s="7"/>
+      <c r="G254" s="7"/>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="3"/>
@@ -8385,12 +8272,8 @@
       <c r="C255" s="9"/>
       <c r="D255" s="6"/>
       <c r="E255" s="6"/>
-      <c r="F255" s="7">
-        <v>10</v>
-      </c>
-      <c r="G255" s="7" t="s">
-        <v>609</v>
-      </c>
+      <c r="F255" s="7"/>
+      <c r="G255" s="7"/>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="3"/>
@@ -8398,12 +8281,8 @@
       <c r="C256" s="9"/>
       <c r="D256" s="6"/>
       <c r="E256" s="6"/>
-      <c r="F256" s="7">
-        <v>11</v>
-      </c>
-      <c r="G256" s="7" t="s">
-        <v>610</v>
-      </c>
+      <c r="F256" s="7"/>
+      <c r="G256" s="7"/>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="3"/>
@@ -8411,12 +8290,8 @@
       <c r="C257" s="9"/>
       <c r="D257" s="6"/>
       <c r="E257" s="6"/>
-      <c r="F257" s="7">
-        <v>12</v>
-      </c>
-      <c r="G257" s="7" t="s">
-        <v>611</v>
-      </c>
+      <c r="F257" s="7"/>
+      <c r="G257" s="7"/>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="3"/>
@@ -8424,12 +8299,8 @@
       <c r="C258" s="9"/>
       <c r="D258" s="6"/>
       <c r="E258" s="6"/>
-      <c r="F258" s="7">
-        <v>13</v>
-      </c>
-      <c r="G258" s="7" t="s">
-        <v>612</v>
-      </c>
+      <c r="F258" s="7"/>
+      <c r="G258" s="7"/>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="3"/>

</xml_diff>

<commit_message>
Corpus Completed Signed-off-by: mashkarharis <mashkarharis@gmail.com>
</commit_message>
<xml_diff>
--- a/song-data-collection/0. Manually Collected Metahpor Data.xlsx
+++ b/song-data-collection/0. Manually Collected Metahpor Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mashk\MyFiles\Semester 7\CS4642 - Data Mining &amp; Information Retrieval\IR-Mini-Project\repo\song-data-collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED5B51F-9E12-49C5-91C7-39C560300BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90820053-CD39-4E51-BC22-B6C7ED3ADFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="635">
   <si>
     <t>ID</t>
   </si>
@@ -1935,6 +1935,9 @@
   </si>
   <si>
     <t>Ravi HaNs | OneStepAhead | Samitha Mudunkotuwa</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -2541,8 +2544,8 @@
   </sheetPr>
   <dimension ref="A1:AD998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E209" workbookViewId="0">
-      <selection activeCell="G232" sqref="G232"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3203,7 +3206,9 @@
       <c r="C26" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>634</v>
+      </c>
       <c r="E26" s="6" t="s">
         <v>84</v>
       </c>
@@ -4237,7 +4242,9 @@
       <c r="C70" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D70" s="6"/>
+      <c r="D70" s="6" t="s">
+        <v>634</v>
+      </c>
       <c r="E70" s="6" t="s">
         <v>624</v>
       </c>
@@ -5522,7 +5529,9 @@
       <c r="C123" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="D123" s="6"/>
+      <c r="D123" s="6" t="s">
+        <v>634</v>
+      </c>
       <c r="E123" s="6" t="s">
         <v>632</v>
       </c>
@@ -5568,7 +5577,9 @@
       <c r="C125" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D125" s="6"/>
+      <c r="D125" s="6" t="s">
+        <v>634</v>
+      </c>
       <c r="E125" s="6" t="s">
         <v>343</v>
       </c>
@@ -5700,7 +5711,9 @@
       <c r="C131" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="D131" s="6"/>
+      <c r="D131" s="6" t="s">
+        <v>634</v>
+      </c>
       <c r="E131" s="6" t="s">
         <v>236</v>
       </c>
@@ -5823,7 +5836,9 @@
       <c r="C136" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="D136" s="6"/>
+      <c r="D136" s="6" t="s">
+        <v>634</v>
+      </c>
       <c r="E136" s="6" t="s">
         <v>370</v>
       </c>
@@ -6646,7 +6661,9 @@
       <c r="C171" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="D171" s="6"/>
+      <c r="D171" s="6" t="s">
+        <v>634</v>
+      </c>
       <c r="E171" s="6" t="s">
         <v>455</v>
       </c>
@@ -6807,7 +6824,9 @@
       <c r="C178" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="D178" s="6"/>
+      <c r="D178" s="6" t="s">
+        <v>634</v>
+      </c>
       <c r="E178" s="6" t="s">
         <v>472</v>
       </c>
@@ -7141,7 +7160,9 @@
       <c r="C192" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="D192" s="6"/>
+      <c r="D192" s="6" t="s">
+        <v>634</v>
+      </c>
       <c r="E192" s="6" t="s">
         <v>503</v>
       </c>
@@ -7657,7 +7678,9 @@
       <c r="C214" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="D214" s="6"/>
+      <c r="D214" s="6" t="s">
+        <v>634</v>
+      </c>
       <c r="E214" s="6" t="s">
         <v>555</v>
       </c>
@@ -8102,10 +8125,7 @@
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B235" s="46"/>
       <c r="C235" s="9"/>
-      <c r="D235" s="7">
-        <f>COUNTBLANK(D2:D233) -122</f>
-        <v>10</v>
-      </c>
+      <c r="D235" s="7"/>
       <c r="I235" s="7"/>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>